<commit_message>
add more race data for pgt samples
</commit_message>
<xml_diff>
--- a/resources/pgt/pgt_sample_metadata.xlsx
+++ b/resources/pgt/pgt_sample_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryan/work/marple/resources/pgt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9F4D12-5320-6142-A28F-69682F62C16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83A8EA0-436F-AE45-B7E0-8F3D9AC9F778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="500" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="383">
   <si>
     <t>accession</t>
   </si>
@@ -1179,6 +1179,12 @@
   </si>
   <si>
     <t>RKBJ</t>
+  </si>
+  <si>
+    <t>RCRS</t>
+  </si>
+  <si>
+    <t>HFCQ</t>
   </si>
 </sst>
 </file>
@@ -1966,7 +1972,7 @@
         <v>83</v>
       </c>
       <c r="G2" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B2,2))</f>
+        <f t="shared" ref="G2:G9" si="0">_xlfn.CONCAT("20", LEFT(B2,2))</f>
         <v>2001</v>
       </c>
       <c r="H2">
@@ -2023,7 +2029,7 @@
         <v>79</v>
       </c>
       <c r="G3" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B3,2))</f>
+        <f t="shared" si="0"/>
         <v>2006</v>
       </c>
       <c r="H3">
@@ -2080,7 +2086,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B4,2))</f>
+        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="H4">
@@ -2137,7 +2143,7 @@
         <v>58</v>
       </c>
       <c r="G5" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B5,2))</f>
+        <f t="shared" si="0"/>
         <v>2007</v>
       </c>
       <c r="H5">
@@ -2194,7 +2200,7 @@
         <v>67</v>
       </c>
       <c r="G6" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B6,2))</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="H6">
@@ -2251,7 +2257,7 @@
         <v>52</v>
       </c>
       <c r="G7" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B7,2))</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="H7">
@@ -2308,7 +2314,7 @@
         <v>54</v>
       </c>
       <c r="G8" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B8,2))</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="H8">
@@ -2365,7 +2371,7 @@
         <v>57</v>
       </c>
       <c r="G9" s="5" t="str">
-        <f>_xlfn.CONCAT("20", LEFT(B9,2))</f>
+        <f t="shared" si="0"/>
         <v>2009</v>
       </c>
       <c r="H9">
@@ -2776,14 +2782,14 @@
         <v>88</v>
       </c>
       <c r="G16" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B16,2))</f>
+        <f t="shared" ref="G16:G39" si="1">_xlfn.CONCAT("19", LEFT(B16,2))</f>
         <v>1956</v>
       </c>
       <c r="H16">
         <v>101</v>
       </c>
       <c r="I16" t="s">
-        <v>103</v>
+        <v>381</v>
       </c>
       <c r="J16" t="s">
         <v>192</v>
@@ -2833,7 +2839,7 @@
         <v>78</v>
       </c>
       <c r="G17" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B17,2))</f>
+        <f t="shared" si="1"/>
         <v>1959</v>
       </c>
       <c r="H17">
@@ -2890,7 +2896,7 @@
         <v>85</v>
       </c>
       <c r="G18" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B18,2))</f>
+        <f t="shared" si="1"/>
         <v>1959</v>
       </c>
       <c r="H18">
@@ -2947,7 +2953,7 @@
         <v>68</v>
       </c>
       <c r="G19" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B19,2))</f>
+        <f t="shared" si="1"/>
         <v>1960</v>
       </c>
       <c r="H19">
@@ -3004,7 +3010,7 @@
         <v>87</v>
       </c>
       <c r="G20" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B20,2))</f>
+        <f t="shared" si="1"/>
         <v>1965</v>
       </c>
       <c r="H20">
@@ -3061,7 +3067,7 @@
         <v>86</v>
       </c>
       <c r="G21" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B21,2))</f>
+        <f t="shared" si="1"/>
         <v>1971</v>
       </c>
       <c r="H21">
@@ -3118,7 +3124,7 @@
         <v>69</v>
       </c>
       <c r="G22" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B22,2))</f>
+        <f t="shared" si="1"/>
         <v>1972</v>
       </c>
       <c r="H22">
@@ -3175,7 +3181,7 @@
         <v>82</v>
       </c>
       <c r="G23" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B23,2))</f>
+        <f t="shared" si="1"/>
         <v>1974</v>
       </c>
       <c r="H23">
@@ -3232,7 +3238,7 @@
         <v>84</v>
       </c>
       <c r="G24" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B24,2))</f>
+        <f t="shared" si="1"/>
         <v>1975</v>
       </c>
       <c r="H24">
@@ -3289,7 +3295,7 @@
         <v>80</v>
       </c>
       <c r="G25" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B25,2))</f>
+        <f t="shared" si="1"/>
         <v>1977</v>
       </c>
       <c r="H25">
@@ -3346,7 +3352,7 @@
         <v>64</v>
       </c>
       <c r="G26" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B26,2))</f>
+        <f t="shared" si="1"/>
         <v>1980</v>
       </c>
       <c r="H26">
@@ -3403,7 +3409,7 @@
         <v>60</v>
       </c>
       <c r="G27" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B27,2))</f>
+        <f t="shared" si="1"/>
         <v>1983</v>
       </c>
       <c r="H27">
@@ -3460,7 +3466,7 @@
         <v>62</v>
       </c>
       <c r="G28" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B28,2))</f>
+        <f t="shared" si="1"/>
         <v>1983</v>
       </c>
       <c r="H28">
@@ -3517,14 +3523,14 @@
         <v>70</v>
       </c>
       <c r="G29" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B29,2))</f>
+        <f t="shared" si="1"/>
         <v>1984</v>
       </c>
       <c r="H29">
         <v>101</v>
       </c>
       <c r="I29" t="s">
-        <v>103</v>
+        <v>382</v>
       </c>
       <c r="J29" t="s">
         <v>192</v>
@@ -3574,7 +3580,7 @@
         <v>76</v>
       </c>
       <c r="G30" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B30,2))</f>
+        <f t="shared" si="1"/>
         <v>1984</v>
       </c>
       <c r="H30">
@@ -3631,7 +3637,7 @@
         <v>71</v>
       </c>
       <c r="G31" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B31,2))</f>
+        <f t="shared" si="1"/>
         <v>1984</v>
       </c>
       <c r="H31">
@@ -3688,7 +3694,7 @@
         <v>75</v>
       </c>
       <c r="G32" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B32,2))</f>
+        <f t="shared" si="1"/>
         <v>1984</v>
       </c>
       <c r="H32">
@@ -3745,7 +3751,7 @@
         <v>63</v>
       </c>
       <c r="G33" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B33,2))</f>
+        <f t="shared" si="1"/>
         <v>1985</v>
       </c>
       <c r="H33">
@@ -3802,7 +3808,7 @@
         <v>66</v>
       </c>
       <c r="G34" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B34,2))</f>
+        <f t="shared" si="1"/>
         <v>1986</v>
       </c>
       <c r="H34">
@@ -3859,7 +3865,7 @@
         <v>77</v>
       </c>
       <c r="G35" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B35,2))</f>
+        <f t="shared" si="1"/>
         <v>1986</v>
       </c>
       <c r="H35">
@@ -3916,7 +3922,7 @@
         <v>65</v>
       </c>
       <c r="G36" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B36,2))</f>
+        <f t="shared" si="1"/>
         <v>1986</v>
       </c>
       <c r="H36">
@@ -3973,7 +3979,7 @@
         <v>61</v>
       </c>
       <c r="G37" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B37,2))</f>
+        <f t="shared" si="1"/>
         <v>1987</v>
       </c>
       <c r="H37">
@@ -4030,7 +4036,7 @@
         <v>74</v>
       </c>
       <c r="G38" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B38,2))</f>
+        <f t="shared" si="1"/>
         <v>1987</v>
       </c>
       <c r="H38">
@@ -4087,7 +4093,7 @@
         <v>59</v>
       </c>
       <c r="G39" s="5" t="str">
-        <f>_xlfn.CONCAT("19", LEFT(B39,2))</f>
+        <f t="shared" si="1"/>
         <v>1996</v>
       </c>
       <c r="H39">

</xml_diff>

<commit_message>
add more race metadata
</commit_message>
<xml_diff>
--- a/resources/pgt/pgt_sample_metadata.xlsx
+++ b/resources/pgt/pgt_sample_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryan/work/marple/resources/pgt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83A8EA0-436F-AE45-B7E0-8F3D9AC9F778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197502A7-E8A3-634F-9852-F742E6A9AC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="500" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="385">
   <si>
     <t>accession</t>
   </si>
@@ -1185,6 +1185,12 @@
   </si>
   <si>
     <t>HFCQ</t>
+  </si>
+  <si>
+    <t>QCCJB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RKQ </t>
   </si>
 </sst>
 </file>
@@ -1873,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5794,7 +5800,7 @@
         <v>150</v>
       </c>
       <c r="I68" t="s">
-        <v>103</v>
+        <v>384</v>
       </c>
       <c r="J68" t="s">
         <v>190</v>
@@ -6773,7 +6779,7 @@
         <v>150</v>
       </c>
       <c r="I85" t="s">
-        <v>103</v>
+        <v>383</v>
       </c>
       <c r="J85" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
add more race metadata to pgt samples
</commit_message>
<xml_diff>
--- a/resources/pgt/pgt_sample_metadata.xlsx
+++ b/resources/pgt/pgt_sample_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryan/work/marple/resources/pgt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197502A7-E8A3-634F-9852-F742E6A9AC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C64DF80-5C79-F24C-A296-C9FECACE4AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21600" yWindow="500" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="391">
   <si>
     <t>accession</t>
   </si>
@@ -1191,6 +1191,24 @@
   </si>
   <si>
     <t xml:space="preserve">RKQ </t>
+  </si>
+  <si>
+    <t>HPCS</t>
+  </si>
+  <si>
+    <t>TMLK</t>
+  </si>
+  <si>
+    <t>MCCD</t>
+  </si>
+  <si>
+    <t>TKRJ</t>
+  </si>
+  <si>
+    <t>GHCS</t>
+  </si>
+  <si>
+    <t>JCMQ</t>
   </si>
 </sst>
 </file>
@@ -1879,7 +1897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2966,7 +2984,7 @@
         <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>385</v>
       </c>
       <c r="J19" t="s">
         <v>192</v>
@@ -3023,7 +3041,7 @@
         <v>101</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>386</v>
       </c>
       <c r="J20" t="s">
         <v>192</v>
@@ -3080,7 +3098,7 @@
         <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>103</v>
+        <v>387</v>
       </c>
       <c r="J21" t="s">
         <v>192</v>
@@ -3251,7 +3269,7 @@
         <v>101</v>
       </c>
       <c r="I24" t="s">
-        <v>103</v>
+        <v>374</v>
       </c>
       <c r="J24" t="s">
         <v>192</v>
@@ -3479,7 +3497,7 @@
         <v>101</v>
       </c>
       <c r="I28" t="s">
-        <v>103</v>
+        <v>388</v>
       </c>
       <c r="J28" t="s">
         <v>192</v>
@@ -3821,7 +3839,7 @@
         <v>101</v>
       </c>
       <c r="I34" t="s">
-        <v>103</v>
+        <v>389</v>
       </c>
       <c r="J34" t="s">
         <v>192</v>
@@ -3992,7 +4010,7 @@
         <v>101</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>390</v>
       </c>
       <c r="J37" t="s">
         <v>192</v>
@@ -5744,7 +5762,7 @@
         <v>101</v>
       </c>
       <c r="I67" t="s">
-        <v>103</v>
+        <v>372</v>
       </c>
       <c r="J67" t="s">
         <v>192</v>

</xml_diff>